<commit_message>
Rerender with final session conts
</commit_message>
<xml_diff>
--- a/SoTL_Compendium_Contributors.xlsx
+++ b/SoTL_Compendium_Contributors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/sotl_glossary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B23D0B-48A6-D244-A8AC-A0F6F6E5DD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75AEDCF6-18AF-F147-9E71-A81F5CC1F1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Order in publication</t>
   </si>
@@ -328,6 +328,9 @@
     <t>Dale</t>
   </si>
   <si>
+    <t>Academic and Digital Development, University of Glasgow</t>
+  </si>
+  <si>
     <t>Ruchi</t>
   </si>
   <si>
@@ -373,7 +376,13 @@
     <t>Stewart</t>
   </si>
   <si>
-    <t>Academic and Digital Development, University of Glasgow</t>
+    <t>Eilidh</t>
+  </si>
+  <si>
+    <t>Soussi</t>
+  </si>
+  <si>
+    <t>School of Education, University of Glasgow</t>
   </si>
 </sst>
 </file>
@@ -798,7 +807,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1163,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
@@ -1179,11 +1188,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" s="7" t="b">
         <v>0</v>
@@ -1228,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
@@ -1245,11 +1254,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="7" t="b">
         <v>0</v>
@@ -1294,13 +1303,13 @@
         <v>0</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="8"/>
       <c r="W7" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="X7" s="7"/>
       <c r="Y7" s="7" t="b">
@@ -1313,11 +1322,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="7" t="b">
         <v>0</v>
@@ -1362,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
@@ -1379,11 +1388,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" s="7" t="b">
         <v>0</v>
@@ -1428,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
@@ -1445,11 +1454,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E10" s="7" t="b">
         <v>0</v>
@@ -1494,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
@@ -1510,9 +1519,13 @@
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E11" s="7" t="b">
         <v>0</v>
       </c>
@@ -1550,12 +1563,14 @@
         <v>0</v>
       </c>
       <c r="Q11" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="S11" s="7"/>
+      <c r="S11" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
       <c r="V11" s="8"/>

</xml_diff>

<commit_message>
definitions updated as of 29th April
</commit_message>
<xml_diff>
--- a/SoTL_Compendium_Contributors.xlsx
+++ b/SoTL_Compendium_Contributors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbartlett/Documents/git_repos/sotl_glossary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/philip_mcaleer_glasgow_ac_uk/Documents/Documents/sotl_glossary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75AEDCF6-18AF-F147-9E71-A81F5CC1F1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{75AEDCF6-18AF-F147-9E71-A81F5CC1F1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0325C26-B76D-4E78-A800-5B3C52C3AEC0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Order in publication</t>
   </si>
@@ -383,6 +383,12 @@
   </si>
   <si>
     <t>School of Education, University of Glasgow</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Draper</t>
   </si>
 </sst>
 </file>
@@ -807,32 +813,32 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="6.5" customWidth="1"/>
-    <col min="13" max="13" width="5.33203125" customWidth="1"/>
-    <col min="14" max="14" width="6.83203125" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" customWidth="1"/>
     <col min="16" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="8.1640625" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" customWidth="1"/>
     <col min="18" max="18" width="9" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" customWidth="1"/>
     <col min="21" max="21" width="11" customWidth="1"/>
-    <col min="22" max="23" width="8.5" customWidth="1"/>
-    <col min="26" max="26" width="12.1640625" customWidth="1"/>
+    <col min="22" max="23" width="8.42578125" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -1585,9 +1591,13 @@
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>57</v>
+      </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="E12" s="7" t="b">
         <v>0</v>
       </c>
@@ -1625,12 +1635,14 @@
         <v>0</v>
       </c>
       <c r="Q12" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="S12" s="7"/>
+      <c r="S12" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="6"/>
@@ -4041,7 +4053,7 @@
       </c>
       <c r="Z52" s="7"/>
     </row>
-    <row r="53" spans="1:26" ht="13">
+    <row r="53" spans="1:26" ht="12.75">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -4101,7 +4113,7 @@
       </c>
       <c r="Z53" s="7"/>
     </row>
-    <row r="54" spans="1:26" ht="13">
+    <row r="54" spans="1:26" ht="12.75">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -4161,7 +4173,7 @@
       </c>
       <c r="Z54" s="7"/>
     </row>
-    <row r="55" spans="1:26" ht="13">
+    <row r="55" spans="1:26" ht="12.75">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -4221,7 +4233,7 @@
       </c>
       <c r="Z55" s="7"/>
     </row>
-    <row r="56" spans="1:26" ht="13">
+    <row r="56" spans="1:26" ht="12.75">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -4281,7 +4293,7 @@
       </c>
       <c r="Z56" s="7"/>
     </row>
-    <row r="57" spans="1:26" ht="13">
+    <row r="57" spans="1:26" ht="12.75">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -4341,7 +4353,7 @@
       </c>
       <c r="Z57" s="7"/>
     </row>
-    <row r="58" spans="1:26" ht="13">
+    <row r="58" spans="1:26" ht="12.75">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -4401,7 +4413,7 @@
       </c>
       <c r="Z58" s="7"/>
     </row>
-    <row r="59" spans="1:26" ht="13">
+    <row r="59" spans="1:26" ht="12.75">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -4461,7 +4473,7 @@
       </c>
       <c r="Z59" s="7"/>
     </row>
-    <row r="60" spans="1:26" ht="13">
+    <row r="60" spans="1:26" ht="12.75">
       <c r="A60" s="7">
         <v>59</v>
       </c>
@@ -4521,7 +4533,7 @@
       </c>
       <c r="Z60" s="7"/>
     </row>
-    <row r="61" spans="1:26" ht="13">
+    <row r="61" spans="1:26" ht="12.75">
       <c r="A61" s="7">
         <v>60</v>
       </c>
@@ -4581,7 +4593,7 @@
       </c>
       <c r="Z61" s="7"/>
     </row>
-    <row r="62" spans="1:26" ht="13">
+    <row r="62" spans="1:26" ht="12.75">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -4641,7 +4653,7 @@
       </c>
       <c r="Z62" s="7"/>
     </row>
-    <row r="63" spans="1:26" ht="13">
+    <row r="63" spans="1:26" ht="12.75">
       <c r="A63" s="7">
         <v>62</v>
       </c>
@@ -4701,7 +4713,7 @@
       </c>
       <c r="Z63" s="7"/>
     </row>
-    <row r="64" spans="1:26" ht="13">
+    <row r="64" spans="1:26" ht="12.75">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -4761,7 +4773,7 @@
       </c>
       <c r="Z64" s="7"/>
     </row>
-    <row r="65" spans="1:26" ht="13">
+    <row r="65" spans="1:26" ht="12.75">
       <c r="A65" s="7">
         <v>64</v>
       </c>
@@ -4821,7 +4833,7 @@
       </c>
       <c r="Z65" s="7"/>
     </row>
-    <row r="66" spans="1:26" ht="13">
+    <row r="66" spans="1:26" ht="12.75">
       <c r="A66" s="7">
         <v>65</v>
       </c>
@@ -4881,7 +4893,7 @@
       </c>
       <c r="Z66" s="7"/>
     </row>
-    <row r="67" spans="1:26" ht="13">
+    <row r="67" spans="1:26" ht="12.75">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -4941,7 +4953,7 @@
       </c>
       <c r="Z67" s="7"/>
     </row>
-    <row r="68" spans="1:26" ht="13">
+    <row r="68" spans="1:26" ht="12.75">
       <c r="A68" s="7">
         <v>67</v>
       </c>
@@ -5001,7 +5013,7 @@
       </c>
       <c r="Z68" s="7"/>
     </row>
-    <row r="69" spans="1:26" ht="13">
+    <row r="69" spans="1:26" ht="12.75">
       <c r="A69" s="7">
         <v>68</v>
       </c>
@@ -5061,7 +5073,7 @@
       </c>
       <c r="Z69" s="7"/>
     </row>
-    <row r="70" spans="1:26" ht="13">
+    <row r="70" spans="1:26" ht="12.75">
       <c r="A70" s="7">
         <v>69</v>
       </c>
@@ -5121,7 +5133,7 @@
       </c>
       <c r="Z70" s="7"/>
     </row>
-    <row r="71" spans="1:26" ht="13">
+    <row r="71" spans="1:26" ht="12.75">
       <c r="A71" s="7">
         <v>70</v>
       </c>
@@ -5181,7 +5193,7 @@
       </c>
       <c r="Z71" s="7"/>
     </row>
-    <row r="72" spans="1:26" ht="13">
+    <row r="72" spans="1:26" ht="12.75">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -5241,7 +5253,7 @@
       </c>
       <c r="Z72" s="7"/>
     </row>
-    <row r="73" spans="1:26" ht="13">
+    <row r="73" spans="1:26" ht="12.75">
       <c r="A73" s="7">
         <v>72</v>
       </c>
@@ -5301,7 +5313,7 @@
       </c>
       <c r="Z73" s="7"/>
     </row>
-    <row r="74" spans="1:26" ht="13">
+    <row r="74" spans="1:26" ht="12.75">
       <c r="A74" s="7">
         <v>73</v>
       </c>
@@ -5361,7 +5373,7 @@
       </c>
       <c r="Z74" s="7"/>
     </row>
-    <row r="75" spans="1:26" ht="13">
+    <row r="75" spans="1:26" ht="12.75">
       <c r="A75" s="7">
         <v>74</v>
       </c>
@@ -5421,7 +5433,7 @@
       </c>
       <c r="Z75" s="7"/>
     </row>
-    <row r="76" spans="1:26" ht="13">
+    <row r="76" spans="1:26" ht="12.75">
       <c r="A76" s="7">
         <v>75</v>
       </c>
@@ -5481,7 +5493,7 @@
       </c>
       <c r="Z76" s="7"/>
     </row>
-    <row r="77" spans="1:26" ht="13">
+    <row r="77" spans="1:26" ht="12.75">
       <c r="A77" s="7">
         <v>76</v>
       </c>
@@ -5541,7 +5553,7 @@
       </c>
       <c r="Z77" s="7"/>
     </row>
-    <row r="78" spans="1:26" ht="13">
+    <row r="78" spans="1:26" ht="12.75">
       <c r="A78" s="7">
         <v>77</v>
       </c>
@@ -5601,7 +5613,7 @@
       </c>
       <c r="Z78" s="7"/>
     </row>
-    <row r="79" spans="1:26" ht="13">
+    <row r="79" spans="1:26" ht="12.75">
       <c r="A79" s="7">
         <v>78</v>
       </c>
@@ -5661,7 +5673,7 @@
       </c>
       <c r="Z79" s="7"/>
     </row>
-    <row r="80" spans="1:26" ht="13">
+    <row r="80" spans="1:26" ht="12.75">
       <c r="A80" s="7">
         <v>79</v>
       </c>
@@ -5721,7 +5733,7 @@
       </c>
       <c r="Z80" s="7"/>
     </row>
-    <row r="81" spans="1:26" ht="13">
+    <row r="81" spans="1:26" ht="12.75">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -5781,7 +5793,7 @@
       </c>
       <c r="Z81" s="7"/>
     </row>
-    <row r="82" spans="1:26" ht="13">
+    <row r="82" spans="1:26" ht="12.75">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -5841,7 +5853,7 @@
       </c>
       <c r="Z82" s="7"/>
     </row>
-    <row r="83" spans="1:26" ht="13">
+    <row r="83" spans="1:26" ht="12.75">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -5901,7 +5913,7 @@
       </c>
       <c r="Z83" s="7"/>
     </row>
-    <row r="84" spans="1:26" ht="13">
+    <row r="84" spans="1:26" ht="12.75">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -5961,7 +5973,7 @@
       </c>
       <c r="Z84" s="7"/>
     </row>
-    <row r="85" spans="1:26" ht="13">
+    <row r="85" spans="1:26" ht="12.75">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -6021,7 +6033,7 @@
       </c>
       <c r="Z85" s="7"/>
     </row>
-    <row r="86" spans="1:26" ht="13">
+    <row r="86" spans="1:26" ht="12.75">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -6081,7 +6093,7 @@
       </c>
       <c r="Z86" s="7"/>
     </row>
-    <row r="87" spans="1:26" ht="13">
+    <row r="87" spans="1:26" ht="12.75">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -6141,7 +6153,7 @@
       </c>
       <c r="Z87" s="7"/>
     </row>
-    <row r="88" spans="1:26" ht="13">
+    <row r="88" spans="1:26" ht="12.75">
       <c r="A88" s="7">
         <v>87</v>
       </c>
@@ -6201,7 +6213,7 @@
       </c>
       <c r="Z88" s="7"/>
     </row>
-    <row r="89" spans="1:26" ht="13">
+    <row r="89" spans="1:26" ht="12.75">
       <c r="A89" s="7">
         <v>88</v>
       </c>
@@ -6261,7 +6273,7 @@
       </c>
       <c r="Z89" s="7"/>
     </row>
-    <row r="90" spans="1:26" ht="13">
+    <row r="90" spans="1:26" ht="12.75">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -6321,7 +6333,7 @@
       </c>
       <c r="Z90" s="7"/>
     </row>
-    <row r="91" spans="1:26" ht="13">
+    <row r="91" spans="1:26" ht="12.75">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -6381,7 +6393,7 @@
       </c>
       <c r="Z91" s="7"/>
     </row>
-    <row r="92" spans="1:26" ht="13">
+    <row r="92" spans="1:26" ht="12.75">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -6441,7 +6453,7 @@
       </c>
       <c r="Z92" s="7"/>
     </row>
-    <row r="93" spans="1:26" ht="13">
+    <row r="93" spans="1:26" ht="12.75">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -6501,7 +6513,7 @@
       </c>
       <c r="Z93" s="7"/>
     </row>
-    <row r="94" spans="1:26" ht="13">
+    <row r="94" spans="1:26" ht="12.75">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -6561,7 +6573,7 @@
       </c>
       <c r="Z94" s="7"/>
     </row>
-    <row r="95" spans="1:26" ht="13">
+    <row r="95" spans="1:26" ht="12.75">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -6621,7 +6633,7 @@
       </c>
       <c r="Z95" s="7"/>
     </row>
-    <row r="96" spans="1:26" ht="13">
+    <row r="96" spans="1:26" ht="12.75">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -6681,7 +6693,7 @@
       </c>
       <c r="Z96" s="7"/>
     </row>
-    <row r="97" spans="1:26" ht="13">
+    <row r="97" spans="1:26" ht="12.75">
       <c r="A97" s="7">
         <v>96</v>
       </c>
@@ -6741,7 +6753,7 @@
       </c>
       <c r="Z97" s="7"/>
     </row>
-    <row r="98" spans="1:26" ht="13">
+    <row r="98" spans="1:26" ht="12.75">
       <c r="A98" s="7">
         <v>97</v>
       </c>
@@ -6801,7 +6813,7 @@
       </c>
       <c r="Z98" s="7"/>
     </row>
-    <row r="99" spans="1:26" ht="13">
+    <row r="99" spans="1:26" ht="12.75">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -6861,7 +6873,7 @@
       </c>
       <c r="Z99" s="7"/>
     </row>
-    <row r="100" spans="1:26" ht="13">
+    <row r="100" spans="1:26" ht="12.75">
       <c r="A100" s="7">
         <v>99</v>
       </c>
@@ -6921,7 +6933,7 @@
       </c>
       <c r="Z100" s="7"/>
     </row>
-    <row r="101" spans="1:26" ht="13">
+    <row r="101" spans="1:26" ht="12.75">
       <c r="A101" s="7">
         <v>100</v>
       </c>

</xml_diff>